<commit_message>
Script de PowerBI, Selección del modelo y de la Predicción del volumen de ampliaciones finalizados.
</commit_message>
<xml_diff>
--- a/Origin_Files/2025.05 Objetivos TELECO INGENIERIA_rev.xlsx
+++ b/Origin_Files/2025.05 Objetivos TELECO INGENIERIA_rev.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UX530\Desktop\MASTER\TFM\Files TMF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UX530\Desktop\TFM-GIT\Origin_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD6DEAB-4EB7-4217-8941-1ABD5B56D235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFF122B-AB57-485C-BF17-C283489B2050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Obj 2024 T1" sheetId="2" r:id="rId1"/>
-    <sheet name="Resumen" sheetId="3" r:id="rId2"/>
+    <sheet name="Obj 2025 T1" sheetId="2" r:id="rId1"/>
+    <sheet name="Resumen Objetivos" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Obj 2024 T1'!$A$5:$P$105</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Obj 2024 T1'!$1:$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Resumen Objetivos'!$A$1:$G$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Obj 2025 T1'!$A$5:$P$105</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Obj 2025 T1'!$1:$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -192,7 +193,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="87">
   <si>
     <t>PROYECTOS</t>
   </si>
@@ -296,9 +297,6 @@
     <t>CONSERVACION EFICIENCIA</t>
   </si>
   <si>
-    <t>PREVISIÓN 2024</t>
-  </si>
-  <si>
     <t>494 INGENIERIA PLANTA EXTERNA- OBJETIVOS</t>
   </si>
   <si>
@@ -431,21 +429,6 @@
     <t>SUBPROYECTO</t>
   </si>
   <si>
-    <t>Suma de Producción Mes+Año</t>
-  </si>
-  <si>
-    <t>Suma de Facturación Mes+Año</t>
-  </si>
-  <si>
-    <t>Suma de Aportación Mes+Año</t>
-  </si>
-  <si>
-    <t>Contratación</t>
-  </si>
-  <si>
-    <t>% Aportación</t>
-  </si>
-  <si>
     <t>Prev Contratación</t>
   </si>
   <si>
@@ -461,28 +444,27 @@
     <t>Prev % Aportación</t>
   </si>
   <si>
-    <t>Coste mes + Año</t>
-  </si>
-  <si>
-    <t>Coste Directo mes + Año</t>
-  </si>
-  <si>
     <t>TELECOMUNICACIONES INGENIERIA - PREV. 2025</t>
   </si>
   <si>
     <t>CIERRE ACUM.MAYO 2025</t>
+  </si>
+  <si>
+    <t>DISEÑO FTTH REDE ABERTA</t>
+  </si>
+  <si>
+    <t>PREVISIÓN 2025</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
   <fonts count="36" x14ac:knownFonts="1">
     <font>
@@ -1202,14 +1184,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="199">
+  <cellXfs count="200">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1772,9 +1753,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1793,25 +1772,19 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="20" fillId="9" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="4">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
-    <cellStyle name="Moneda" xfId="4" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -2178,8 +2151,8 @@
   <dimension ref="A1:AL107"/>
   <sheetViews>
     <sheetView showGridLines="0" showZeros="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -2200,22 +2173,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="193" t="s">
-        <v>91</v>
-      </c>
-      <c r="B1" s="194"/>
-      <c r="C1" s="194"/>
-      <c r="D1" s="194"/>
-      <c r="E1" s="194"/>
-      <c r="F1" s="194"/>
-      <c r="G1" s="194"/>
-      <c r="H1" s="194"/>
-      <c r="I1" s="194"/>
-      <c r="J1" s="194"/>
-      <c r="K1" s="194"/>
-      <c r="L1" s="194"/>
-      <c r="M1" s="194"/>
-      <c r="N1" s="194"/>
+      <c r="A1" s="191" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="192"/>
+      <c r="C1" s="192"/>
+      <c r="D1" s="192"/>
+      <c r="E1" s="192"/>
+      <c r="F1" s="192"/>
+      <c r="G1" s="192"/>
+      <c r="H1" s="192"/>
+      <c r="I1" s="192"/>
+      <c r="J1" s="192"/>
+      <c r="K1" s="192"/>
+      <c r="L1" s="192"/>
+      <c r="M1" s="192"/>
+      <c r="N1" s="192"/>
       <c r="O1" s="21" t="s">
         <v>10</v>
       </c>
@@ -2224,33 +2197,33 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="35.4" x14ac:dyDescent="0.25">
-      <c r="A2" s="195" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="197" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="197"/>
-      <c r="D2" s="197"/>
-      <c r="E2" s="197"/>
-      <c r="F2" s="197"/>
-      <c r="G2" s="197" t="s">
-        <v>92</v>
-      </c>
-      <c r="H2" s="197"/>
-      <c r="I2" s="197"/>
-      <c r="J2" s="197"/>
-      <c r="K2" s="197"/>
-      <c r="L2" s="197" t="s">
+      <c r="A2" s="193" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="195" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="195"/>
+      <c r="D2" s="195"/>
+      <c r="E2" s="195"/>
+      <c r="F2" s="195"/>
+      <c r="G2" s="195" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="195"/>
+      <c r="I2" s="195"/>
+      <c r="J2" s="195"/>
+      <c r="K2" s="195"/>
+      <c r="L2" s="195" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="197"/>
-      <c r="N2" s="197"/>
-      <c r="O2" s="197"/>
-      <c r="P2" s="198"/>
+      <c r="M2" s="195"/>
+      <c r="N2" s="195"/>
+      <c r="O2" s="195"/>
+      <c r="P2" s="196"/>
     </row>
     <row r="3" spans="1:16" s="6" customFormat="1" ht="48.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="196"/>
+      <c r="A3" s="194"/>
       <c r="B3" s="9" t="s">
         <v>9</v>
       </c>
@@ -2299,7 +2272,7 @@
     </row>
     <row r="4" spans="1:16" s="20" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="32">
         <f>B5+B34</f>
@@ -2364,7 +2337,7 @@
     </row>
     <row r="5" spans="1:16" s="20" customFormat="1" ht="29.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="36">
         <v>3400</v>
@@ -2522,7 +2495,7 @@
         <v>15.154960000000044</v>
       </c>
       <c r="K7" s="130">
-        <f t="shared" si="3"/>
+        <f>J7/H7</f>
         <v>4.1519912816446118E-2</v>
       </c>
       <c r="L7" s="44">
@@ -2728,8 +2701,8 @@
       </c>
     </row>
     <row r="11" spans="1:16" s="20" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="52" t="s">
-        <v>37</v>
+      <c r="A11" s="197" t="s">
+        <v>36</v>
       </c>
       <c r="B11" s="53">
         <f>C11</f>
@@ -2847,7 +2820,7 @@
     </row>
     <row r="13" spans="1:16" s="20" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="52" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="53">
         <v>550</v>
@@ -3026,7 +2999,7 @@
     </row>
     <row r="16" spans="1:16" s="20" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="52" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B16" s="53">
         <f>C16</f>
@@ -3144,7 +3117,7 @@
     </row>
     <row r="18" spans="1:16" s="20" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="52" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18" s="44">
         <f>C18</f>
@@ -3203,7 +3176,7 @@
     </row>
     <row r="19" spans="1:16" s="20" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="52" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B19" s="44">
         <f>C19</f>
@@ -3262,7 +3235,7 @@
     </row>
     <row r="20" spans="1:16" s="20" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="52" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" s="57">
         <v>140</v>
@@ -3385,7 +3358,7 @@
     </row>
     <row r="22" spans="1:16" s="20" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="52" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="B22" s="60">
         <v>220</v>
@@ -3461,7 +3434,7 @@
     </row>
     <row r="24" spans="1:16" s="20" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="108" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B24" s="63"/>
       <c r="C24" s="64"/>
@@ -3499,7 +3472,7 @@
     </row>
     <row r="25" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="109" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B25" s="28">
         <v>0.13</v>
@@ -3544,7 +3517,7 @@
     </row>
     <row r="26" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="109" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B26" s="28"/>
       <c r="C26" s="30"/>
@@ -3584,7 +3557,7 @@
     </row>
     <row r="27" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="109" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B27" s="28"/>
       <c r="C27" s="30"/>
@@ -3626,7 +3599,7 @@
     </row>
     <row r="28" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="109" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B28" s="28"/>
       <c r="C28" s="30"/>
@@ -3668,7 +3641,7 @@
     </row>
     <row r="29" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="109" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B29" s="28"/>
       <c r="C29" s="30"/>
@@ -3720,7 +3693,7 @@
     </row>
     <row r="30" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="109" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B30" s="28"/>
       <c r="C30" s="30"/>
@@ -3757,7 +3730,7 @@
     </row>
     <row r="31" spans="1:16" s="20" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="66" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B31" s="67"/>
       <c r="C31" s="68"/>
@@ -3785,7 +3758,7 @@
     </row>
     <row r="32" spans="1:16" s="20" customFormat="1" ht="29.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="71" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B32" s="72">
         <f>B6+B15+B10+B21</f>
@@ -3906,7 +3879,7 @@
     </row>
     <row r="34" spans="1:16" s="20" customFormat="1" ht="29.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B34" s="36">
         <f>B48</f>
@@ -3968,7 +3941,7 @@
     </row>
     <row r="35" spans="1:16" s="20" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B35" s="41">
         <v>1800</v>
@@ -4029,7 +4002,7 @@
     </row>
     <row r="36" spans="1:16" s="20" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="52" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B36" s="53">
         <v>1000</v>
@@ -4087,7 +4060,7 @@
     </row>
     <row r="37" spans="1:16" s="20" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="52" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B37" s="53">
         <v>800</v>
@@ -4144,7 +4117,7 @@
     </row>
     <row r="38" spans="1:16" s="20" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="52" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B38" s="53"/>
       <c r="C38" s="54"/>
@@ -4226,7 +4199,7 @@
     </row>
     <row r="40" spans="1:16" s="20" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="111" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B40" s="64"/>
       <c r="C40" s="64"/>
@@ -4264,7 +4237,7 @@
     </row>
     <row r="41" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="109" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B41" s="28">
         <v>0.13</v>
@@ -4307,7 +4280,7 @@
     </row>
     <row r="42" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="109" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B42" s="28"/>
       <c r="C42" s="30"/>
@@ -4349,7 +4322,7 @@
     </row>
     <row r="43" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="109" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B43" s="28"/>
       <c r="C43" s="30"/>
@@ -4391,7 +4364,7 @@
     </row>
     <row r="44" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="109" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B44" s="28"/>
       <c r="C44" s="30"/>
@@ -4433,7 +4406,7 @@
     </row>
     <row r="45" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="109" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B45" s="28"/>
       <c r="C45" s="30"/>
@@ -4485,7 +4458,7 @@
     </row>
     <row r="46" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="109" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B46" s="28"/>
       <c r="C46" s="30"/>
@@ -4527,7 +4500,7 @@
     </row>
     <row r="47" spans="1:16" s="20" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="66" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B47" s="67"/>
       <c r="C47" s="68"/>
@@ -4563,7 +4536,7 @@
     </row>
     <row r="48" spans="1:16" s="20" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="71" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48" s="72">
         <f>B36+B37+B38</f>
@@ -4702,7 +4675,7 @@
     </row>
     <row r="51" spans="1:16" s="20" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="81" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B51" s="82">
         <f>B32+B48</f>
@@ -4841,7 +4814,7 @@
     </row>
     <row r="54" spans="1:16" s="117" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B54" s="33">
         <f>B55+B86</f>
@@ -4906,7 +4879,7 @@
     </row>
     <row r="55" spans="1:16" s="7" customFormat="1" ht="29.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B55" s="36">
         <v>4600</v>
@@ -5322,7 +5295,7 @@
     </row>
     <row r="62" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B62" s="40">
         <f>SUM(B63:B67)</f>
@@ -5387,7 +5360,7 @@
     </row>
     <row r="63" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="52" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B63" s="23">
         <v>165</v>
@@ -5677,7 +5650,7 @@
     </row>
     <row r="68" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B68" s="40">
         <f>SUM(B69:B70)</f>
@@ -5980,7 +5953,7 @@
     </row>
     <row r="73" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B73" s="40">
         <f>SUM(B74:B74)</f>
@@ -6045,7 +6018,7 @@
     </row>
     <row r="74" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="43" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B74" s="14">
         <v>300</v>
@@ -6133,7 +6106,7 @@
     </row>
     <row r="76" spans="1:16" s="1" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="108" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B76" s="63"/>
       <c r="C76" s="64"/>
@@ -6171,7 +6144,7 @@
     </row>
     <row r="77" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="109" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B77" s="28">
         <v>0.115</v>
@@ -6214,7 +6187,7 @@
     </row>
     <row r="78" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="109" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B78" s="28"/>
       <c r="C78" s="30"/>
@@ -6256,7 +6229,7 @@
     </row>
     <row r="79" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="109" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B79" s="28"/>
       <c r="C79" s="30"/>
@@ -6299,7 +6272,7 @@
     </row>
     <row r="80" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="109" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B80" s="28"/>
       <c r="C80" s="30"/>
@@ -6342,7 +6315,7 @@
     </row>
     <row r="81" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="109" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B81" s="28"/>
       <c r="C81" s="30"/>
@@ -6396,7 +6369,7 @@
     </row>
     <row r="82" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="109" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B82" s="28"/>
       <c r="C82" s="30"/>
@@ -6436,7 +6409,7 @@
     </row>
     <row r="83" spans="1:16" s="7" customFormat="1" ht="29.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="71" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B83" s="72">
         <f>B56+B62+B68+B73+B71</f>
@@ -6575,7 +6548,7 @@
     </row>
     <row r="86" spans="1:16" s="116" customFormat="1" ht="29.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="114" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B86" s="32">
         <v>4200</v>
@@ -6701,7 +6674,7 @@
     </row>
     <row r="88" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B88" s="23">
         <v>2800</v>
@@ -6759,7 +6732,7 @@
     </row>
     <row r="89" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="52" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B89" s="11">
         <v>1250</v>
@@ -6817,7 +6790,7 @@
     </row>
     <row r="90" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="43" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B90" s="11">
         <v>100</v>
@@ -6875,7 +6848,7 @@
     </row>
     <row r="91" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="43" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B91" s="11">
         <v>50</v>
@@ -6951,7 +6924,7 @@
     </row>
     <row r="93" spans="1:16" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="108" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B93" s="97"/>
       <c r="C93" s="98"/>
@@ -6989,7 +6962,7 @@
     </row>
     <row r="94" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="109" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B94" s="28">
         <v>0.105</v>
@@ -7032,7 +7005,7 @@
     </row>
     <row r="95" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="109" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B95" s="28"/>
       <c r="C95" s="30"/>
@@ -7074,7 +7047,7 @@
     </row>
     <row r="96" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="109" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B96" s="28"/>
       <c r="C96" s="30"/>
@@ -7117,7 +7090,7 @@
     </row>
     <row r="97" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="109" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B97" s="28"/>
       <c r="C97" s="30"/>
@@ -7159,7 +7132,7 @@
     </row>
     <row r="98" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="109" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B98" s="28"/>
       <c r="C98" s="30"/>
@@ -7209,7 +7182,7 @@
     </row>
     <row r="99" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="109" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B99" s="28"/>
       <c r="C99" s="30"/>
@@ -7276,7 +7249,7 @@
     </row>
     <row r="101" spans="1:16" s="1" customFormat="1" ht="29.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="71" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B101" s="72">
         <f>B87</f>
@@ -7397,7 +7370,7 @@
     </row>
     <row r="103" spans="1:16" s="1" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="81" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B103" s="82">
         <f>B83+B101</f>
@@ -7518,7 +7491,7 @@
     </row>
     <row r="105" spans="1:16" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="99" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B105" s="100">
         <f>B4+B54</f>
@@ -7583,7 +7556,7 @@
     </row>
     <row r="106" spans="1:16" s="5" customFormat="1" ht="44.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="102" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B106" s="103">
         <f>B51+B103</f>
@@ -7648,7 +7621,7 @@
     </row>
     <row r="107" spans="1:16" s="27" customFormat="1" ht="31.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="105" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B107" s="106">
         <f>+B106/B105</f>
@@ -7707,62 +7680,62 @@
     <mergeCell ref="L2:P2"/>
   </mergeCells>
   <conditionalFormatting sqref="F5:F50">
-    <cfRule type="cellIs" dxfId="12" priority="55" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="55" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F53:F83">
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F85:F102">
-    <cfRule type="cellIs" dxfId="10" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="15" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F105:F107">
-    <cfRule type="cellIs" dxfId="9" priority="98" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="98" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:K50">
-    <cfRule type="cellIs" dxfId="8" priority="49" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="49" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K53:K83">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K85:K102">
-    <cfRule type="cellIs" dxfId="6" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K105:K107">
-    <cfRule type="cellIs" dxfId="5" priority="84" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="84" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P50">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P53:P83">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P85:P102">
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P105:P107">
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7778,675 +7751,367 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N14"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B8:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.26953125" customWidth="1"/>
     <col min="2" max="2" width="30.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.90625" style="198" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.54296875" style="198" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.08984375" style="198" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" style="198" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.81640625" style="190" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" t="s">
         <v>77</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="198" t="s">
         <v>78</v>
       </c>
-      <c r="C1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="D1" s="198" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="198" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="198" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="190" t="s">
         <v>82</v>
       </c>
-      <c r="I1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J1" t="s">
-        <v>80</v>
-      </c>
-      <c r="K1" t="s">
-        <v>81</v>
-      </c>
-      <c r="L1" s="189" t="s">
-        <v>83</v>
-      </c>
-      <c r="M1" t="s">
-        <v>89</v>
-      </c>
-      <c r="N1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="190">
+        <v>38</v>
+      </c>
+      <c r="C2" s="199">
         <v>60000</v>
       </c>
-      <c r="D2" s="190">
+      <c r="D2" s="199">
         <v>60000</v>
       </c>
-      <c r="E2" s="190">
+      <c r="E2" s="199">
         <v>60000</v>
       </c>
-      <c r="F2" s="190">
+      <c r="F2" s="199">
         <v>3000</v>
       </c>
       <c r="G2" s="189">
         <f>F2/D2</f>
         <v>0.05</v>
       </c>
-      <c r="H2" s="190">
-        <v>53588</v>
-      </c>
-      <c r="I2" s="190">
-        <v>53588</v>
-      </c>
-      <c r="J2" s="190">
-        <v>44341</v>
-      </c>
-      <c r="K2" s="190">
-        <v>2990</v>
-      </c>
-      <c r="L2" s="191">
-        <f t="shared" ref="L2:L14" si="0">K2/I2</f>
-        <v>5.5796073747853996E-2</v>
-      </c>
-      <c r="M2" s="192">
-        <v>45097.000000000007</v>
-      </c>
-      <c r="N2" s="192">
-        <v>37450</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="190">
+        <v>39</v>
+      </c>
+      <c r="C3" s="199">
         <v>20000</v>
       </c>
-      <c r="D3" s="190">
+      <c r="D3" s="199">
         <v>20000</v>
       </c>
-      <c r="E3" s="190">
+      <c r="E3" s="199">
         <v>20000</v>
       </c>
-      <c r="F3" s="190">
+      <c r="F3" s="199">
         <v>2000</v>
       </c>
       <c r="G3" s="189">
-        <f t="shared" ref="G3:G14" si="1">F3/D3</f>
+        <f t="shared" ref="G3:G14" si="0">F3/D3</f>
         <v>0.1</v>
       </c>
-      <c r="H3" s="190">
-        <v>14500</v>
-      </c>
-      <c r="I3" s="190">
-        <v>14500</v>
-      </c>
-      <c r="J3" s="190">
-        <v>0</v>
-      </c>
-      <c r="K3" s="190">
-        <v>610</v>
-      </c>
-      <c r="L3" s="191">
-        <f t="shared" si="0"/>
-        <v>4.2068965517241382E-2</v>
-      </c>
-      <c r="M3" s="192">
-        <v>16285.24</v>
-      </c>
-      <c r="N3" s="192">
-        <v>14216.09</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="190">
+      <c r="C4" s="199">
         <v>60000</v>
       </c>
-      <c r="D4" s="190">
+      <c r="D4" s="199">
         <v>60000</v>
       </c>
-      <c r="E4" s="190">
+      <c r="E4" s="199">
         <v>60000</v>
       </c>
-      <c r="F4" s="190">
+      <c r="F4" s="199">
         <v>6000</v>
       </c>
       <c r="G4" s="189">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="H4" s="190">
-        <v>15450</v>
-      </c>
-      <c r="I4" s="190">
-        <v>15450</v>
-      </c>
-      <c r="J4" s="190">
-        <v>14250</v>
-      </c>
-      <c r="K4" s="190">
-        <v>-11050</v>
-      </c>
-      <c r="L4" s="191">
-        <f t="shared" si="0"/>
-        <v>-0.71521035598705507</v>
-      </c>
-      <c r="M4" s="192">
-        <v>24468.91</v>
-      </c>
-      <c r="N4" s="192">
-        <v>22435.48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="190">
+        <v>41</v>
+      </c>
+      <c r="C5" s="199">
         <v>140000</v>
       </c>
-      <c r="D5" s="190">
+      <c r="D5" s="199">
         <v>100000</v>
       </c>
-      <c r="E5" s="190">
+      <c r="E5" s="199">
         <v>100000</v>
       </c>
-      <c r="F5" s="190">
+      <c r="F5" s="199">
         <v>8000</v>
       </c>
       <c r="G5" s="189">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
-      <c r="H5" s="190">
-        <v>38750</v>
-      </c>
-      <c r="I5" s="190">
-        <v>38750</v>
-      </c>
-      <c r="J5" s="190">
-        <v>47470</v>
-      </c>
-      <c r="K5" s="190">
-        <v>-16170</v>
-      </c>
-      <c r="L5" s="191">
-        <f t="shared" si="0"/>
-        <v>-0.41729032258064513</v>
-      </c>
-      <c r="M5" s="192">
-        <v>6835.92</v>
-      </c>
-      <c r="N5" s="192">
-        <v>6835.92</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="190">
+        <v>40</v>
+      </c>
+      <c r="C6" s="199">
         <v>10000</v>
       </c>
-      <c r="D6" s="190">
+      <c r="D6" s="199">
         <v>10000</v>
       </c>
-      <c r="E6" s="190">
+      <c r="E6" s="199">
         <v>10000</v>
       </c>
-      <c r="F6" s="190">
+      <c r="F6" s="199">
         <v>1000</v>
       </c>
       <c r="G6" s="189">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="H6" s="190">
-        <v>2521.3599999999997</v>
-      </c>
-      <c r="I6" s="190">
-        <v>2521.3599999999997</v>
-      </c>
-      <c r="J6" s="190">
-        <v>2758.8599999999997</v>
-      </c>
-      <c r="K6" s="190">
-        <v>260</v>
-      </c>
-      <c r="L6" s="191">
-        <f t="shared" si="0"/>
-        <v>0.10311895167687281</v>
-      </c>
-      <c r="M6" s="192">
-        <v>859.8</v>
-      </c>
-      <c r="N6" s="192">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
       <c r="B7" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="190">
+      <c r="C7" s="199">
         <v>200000</v>
       </c>
-      <c r="D7" s="190">
+      <c r="D7" s="199">
         <v>200000</v>
       </c>
-      <c r="E7" s="190">
+      <c r="E7" s="199">
         <v>200000</v>
       </c>
-      <c r="F7" s="190">
+      <c r="F7" s="199">
         <v>2000</v>
       </c>
       <c r="G7" s="189">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="H7" s="190">
-        <v>64850</v>
-      </c>
-      <c r="I7" s="190">
-        <v>64850</v>
-      </c>
-      <c r="J7" s="190">
-        <v>64260</v>
-      </c>
-      <c r="K7" s="190">
-        <v>-33980</v>
-      </c>
-      <c r="L7" s="191">
-        <f t="shared" si="0"/>
-        <v>-0.52397841171935233</v>
-      </c>
-      <c r="M7" s="192">
-        <v>84325.25</v>
-      </c>
-      <c r="N7" s="192">
-        <v>73661.06</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="190">
+        <v>36</v>
+      </c>
+      <c r="C8" s="199">
         <v>220000</v>
       </c>
-      <c r="D8" s="190">
+      <c r="D8" s="199">
         <v>220000</v>
       </c>
-      <c r="E8" s="190">
+      <c r="E8" s="199">
         <v>220000</v>
       </c>
-      <c r="F8" s="190">
+      <c r="F8" s="199">
         <v>15000</v>
       </c>
       <c r="G8" s="189">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6.8181818181818177E-2</v>
       </c>
-      <c r="H8" s="190">
-        <v>105962.48999999999</v>
-      </c>
-      <c r="I8" s="190">
-        <v>105962.48999999999</v>
-      </c>
-      <c r="J8" s="190">
-        <v>105200</v>
-      </c>
-      <c r="K8" s="190">
-        <v>7140</v>
-      </c>
-      <c r="L8" s="191">
-        <f t="shared" si="0"/>
-        <v>6.7382335013078692E-2</v>
-      </c>
-      <c r="M8" s="192">
-        <v>91821.25</v>
-      </c>
-      <c r="N8" s="192">
-        <v>76700.41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="190">
+        <v>37</v>
+      </c>
+      <c r="C9" s="199">
         <v>550000</v>
       </c>
-      <c r="D9" s="190">
+      <c r="D9" s="199">
         <v>460000</v>
       </c>
-      <c r="E9" s="190">
+      <c r="E9" s="199">
         <v>460000</v>
       </c>
-      <c r="F9" s="190">
+      <c r="F9" s="199">
         <v>33000</v>
       </c>
       <c r="G9" s="189">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7.1739130434782611E-2</v>
       </c>
-      <c r="H9" s="190">
-        <v>90000</v>
-      </c>
-      <c r="I9" s="190">
-        <v>10880</v>
-      </c>
-      <c r="J9" s="190">
-        <v>0</v>
-      </c>
-      <c r="K9" s="190">
-        <v>-9860</v>
-      </c>
-      <c r="L9" s="191">
-        <f t="shared" si="0"/>
-        <v>-0.90625</v>
-      </c>
-      <c r="M9" s="192">
-        <v>0</v>
-      </c>
-      <c r="N9" s="192">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="190">
+      <c r="C10" s="199">
         <v>600000</v>
       </c>
-      <c r="D10" s="190">
+      <c r="D10" s="199">
         <v>600000</v>
       </c>
-      <c r="E10" s="190">
+      <c r="E10" s="199">
         <v>600000</v>
       </c>
-      <c r="F10" s="190">
+      <c r="F10" s="199">
         <v>77600</v>
       </c>
       <c r="G10" s="189">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.12933333333333333</v>
       </c>
-      <c r="H10" s="190">
-        <v>497650</v>
-      </c>
-      <c r="I10" s="190">
-        <v>462050</v>
-      </c>
-      <c r="J10" s="190">
-        <v>475900</v>
-      </c>
-      <c r="K10" s="190">
-        <v>58270</v>
-      </c>
-      <c r="L10" s="191">
-        <f t="shared" si="0"/>
-        <v>0.12611189265231035</v>
-      </c>
-      <c r="M10" s="192">
-        <v>400378.94</v>
-      </c>
-      <c r="N10" s="192">
-        <v>334301.7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
       <c r="B11" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="190">
+      <c r="C11" s="199">
         <v>220000</v>
       </c>
-      <c r="D11" s="190">
+      <c r="D11" s="199">
         <v>160000</v>
       </c>
-      <c r="E11" s="190">
+      <c r="E11" s="199">
         <v>160000</v>
       </c>
-      <c r="F11" s="190">
+      <c r="F11" s="199">
         <v>20000</v>
       </c>
       <c r="G11" s="189">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
-      <c r="H11" s="190">
-        <v>198552.25</v>
-      </c>
-      <c r="I11" s="190">
-        <v>198552.25</v>
-      </c>
-      <c r="J11" s="190">
-        <v>155754.25</v>
-      </c>
-      <c r="K11" s="190">
-        <v>64107.889999999985</v>
-      </c>
-      <c r="L11" s="191">
-        <f t="shared" si="0"/>
-        <v>0.32287667352044608</v>
-      </c>
-      <c r="M11" s="192">
-        <v>134444.36000000002</v>
-      </c>
-      <c r="N11" s="192">
-        <v>106110.96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="190">
+      <c r="C12" s="199">
         <v>450000</v>
       </c>
-      <c r="D12" s="190">
+      <c r="D12" s="199">
         <v>410000</v>
       </c>
-      <c r="E12" s="190">
+      <c r="E12" s="199">
         <v>410000</v>
       </c>
-      <c r="F12" s="190">
+      <c r="F12" s="199">
         <v>76200</v>
       </c>
       <c r="G12" s="189">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.18585365853658536</v>
       </c>
-      <c r="H12" s="190">
-        <v>173190.21000000002</v>
-      </c>
-      <c r="I12" s="190">
-        <v>173190.21000000002</v>
-      </c>
-      <c r="J12" s="190">
-        <v>173447.84</v>
-      </c>
-      <c r="K12" s="190">
-        <v>30260</v>
-      </c>
-      <c r="L12" s="191">
-        <f t="shared" si="0"/>
-        <v>0.1747211923814862</v>
-      </c>
-      <c r="M12" s="192">
-        <v>152934.12</v>
-      </c>
-      <c r="N12" s="192">
-        <v>128219.87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
       <c r="B13" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="190">
+      <c r="C13" s="199">
         <v>500000</v>
       </c>
-      <c r="D13" s="190">
+      <c r="D13" s="199">
         <v>450000</v>
       </c>
-      <c r="E13" s="190">
+      <c r="E13" s="199">
         <v>450000</v>
       </c>
-      <c r="F13" s="190">
+      <c r="F13" s="199">
         <v>30000</v>
       </c>
       <c r="G13" s="189">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="H13" s="190">
-        <v>365004.62</v>
-      </c>
-      <c r="I13" s="190">
-        <v>365004.62</v>
-      </c>
-      <c r="J13" s="190">
-        <v>322286.5</v>
-      </c>
-      <c r="K13" s="190">
-        <v>15150</v>
-      </c>
-      <c r="L13" s="191">
-        <f t="shared" si="0"/>
-        <v>4.1506323947351681E-2</v>
-      </c>
-      <c r="M13" s="192">
-        <v>364849.66</v>
-      </c>
-      <c r="N13" s="192">
-        <v>312763.50000000006</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="190">
+      <c r="C14" s="199">
         <v>370000</v>
       </c>
-      <c r="D14" s="190">
+      <c r="D14" s="199">
         <v>350000</v>
       </c>
-      <c r="E14" s="190">
+      <c r="E14" s="199">
         <v>350000</v>
       </c>
-      <c r="F14" s="190">
+      <c r="F14" s="199">
         <v>61200</v>
       </c>
       <c r="G14" s="189">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.17485714285714285</v>
       </c>
-      <c r="H14" s="190">
-        <v>189512.78</v>
-      </c>
-      <c r="I14" s="190">
-        <v>189512.78</v>
-      </c>
-      <c r="J14" s="190">
-        <v>203931.25999999998</v>
-      </c>
-      <c r="K14" s="190">
-        <v>20470</v>
-      </c>
-      <c r="L14" s="191">
-        <f t="shared" si="0"/>
-        <v>0.10801382365875273</v>
-      </c>
-      <c r="M14" s="192">
-        <v>133394.48000000001</v>
-      </c>
-      <c r="N14" s="192">
-        <v>106351</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="L1:L14">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
+  <autoFilter ref="A1:G14" xr:uid="{00000000-0001-0000-0100-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="MASMOVIL"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>